<commit_message>
added code for multithreading
</commit_message>
<xml_diff>
--- a/BasicProgramLearn/needful/Book1.xlsx
+++ b/BasicProgramLearn/needful/Book1.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Emp Id</t>
   </si>
@@ -54,14 +55,121 @@
   </si>
   <si>
     <t>Saiva</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>null,null</t>
+  </si>
+  <si>
+    <t>24,30</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>SSH.RowCnt</t>
+  </si>
+  <si>
+    <t>SSH.SubScriptionID</t>
+  </si>
+  <si>
+    <t>SSH.SubScribeTypeID</t>
+  </si>
+  <si>
+    <t>SSH.ClientIp</t>
+  </si>
+  <si>
+    <t>SSH.TrackingCodeID</t>
+  </si>
+  <si>
+    <t>SSH.SubscribeSourceID</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>null,null,null</t>
+  </si>
+  <si>
+    <t>15,15</t>
+  </si>
+  <si>
+    <t>5,5</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>24.193.86.57,24.193.86.57</t>
+  </si>
+  <si>
+    <t>28,28</t>
+  </si>
+  <si>
+    <t>24.193.86.57</t>
+  </si>
+  <si>
+    <t>11,17</t>
+  </si>
+  <si>
+    <t>108,15,121</t>
+  </si>
+  <si>
+    <t>1,5,5</t>
+  </si>
+  <si>
+    <t>24.193.86.57,24.193.86.57,24.193.86.57</t>
+  </si>
+  <si>
+    <t>28,28,48</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Context</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -89,8 +197,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -470,4 +585,150 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>